<commit_message>
absolute path centric label tree and statistic
</commit_message>
<xml_diff>
--- a/Server/statistic/Say Thank You.xlsx
+++ b/Server/statistic/Say Thank You.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Text</t>
   </si>
@@ -25,40 +25,43 @@
     <t>Count</t>
   </si>
   <si>
+    <t xml:space="preserve">someone </t>
+  </si>
+  <si>
+    <t>ape-thief</t>
+  </si>
+  <si>
+    <t>woman</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> gorilla</t>
+  </si>
+  <si>
+    <t>that</t>
+  </si>
+  <si>
+    <t>batman</t>
+  </si>
+  <si>
     <t>someone</t>
   </si>
   <si>
-    <t>ape-thief</t>
-  </si>
-  <si>
-    <t>bane</t>
-  </si>
-  <si>
-    <t>going</t>
-  </si>
-  <si>
-    <t>big bat</t>
-  </si>
-  <si>
-    <t>batman</t>
-  </si>
-  <si>
-    <t>Per</t>
-  </si>
-  <si>
-    <t>Agent</t>
-  </si>
-  <si>
-    <t>Trigger</t>
-  </si>
-  <si>
-    <t>Veh</t>
-  </si>
-  <si>
-    <t>Wea</t>
-  </si>
-  <si>
-    <t>Gpe</t>
+    <t>root_Entity_Per_Per</t>
+  </si>
+  <si>
+    <t>root_Event_Life_Be-Born_Trigger</t>
+  </si>
+  <si>
+    <t>root_Event_Life_Marry_Trigger</t>
+  </si>
+  <si>
+    <t>root_Event_Life_Marry_Person</t>
+  </si>
+  <si>
+    <t>root_Event_Life_Marry_Place</t>
+  </si>
+  <si>
+    <t>root_Entity_Veh_Veh</t>
   </si>
 </sst>
 </file>
@@ -438,10 +441,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -449,7 +452,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -460,7 +463,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -471,7 +474,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -482,10 +485,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -493,7 +496,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -501,10 +504,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>1</v>

</xml_diff>